<commit_message>
update(232 baterias ion litio iniciales)
</commit_message>
<xml_diff>
--- a/baterias_iniciales.xlsx
+++ b/baterias_iniciales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ce3gk\OneDrive\Escritorio\opti\proyecto\ics1113_proyecto_grupo03\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\OneDrive\Documentos\UC\Semester 6\OPTI\tarea\Proyecto\ics1113_proyecto_grupo03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D577B67C-920E-40B0-B004-0CB76BE67D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFE8F75-3567-49E4-9F22-263CFF42145B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="b0" sheetId="1" r:id="rId1"/>
@@ -418,9 +418,9 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -436,7 +436,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -454,12 +454,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,15 +467,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>

</xml_diff>